<commit_message>
Various content and style updates
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -17,7 +17,7 @@
 Columns: Qualitative outcomes</t>
   </si>
   <si>
-    <t>Summary / highlights</t>
+    <t>Development Stage Summary</t>
   </si>
   <si>
     <t>Malicious use</t>
@@ -44,7 +44,7 @@
     <t>Bonus notes</t>
   </si>
   <si>
-    <t>Summary</t>
+    <t>Qualitative Outcome Summary</t>
   </si>
   <si>
     <t>Pretraining creates capabilities that malicious actors may want to elicit. Harmlessness finetuning makes it somewhat difficult to elicit them towards harmful purposes, but it’s never all that difficult (so far). With finetuning access, malicious actors can undo harmlessness training and make models more willing to act on harmful requests. Refusal vector ablation is another intervention that can remove harmlessness if the malicious user has whitebox access. Harmful behavior is ultimately elicited by making harmful requests that the models don’t refuse, perhaps because of the vulnerabilities described above or things like adversarial input suffixes. A harmful input may also come from a third-party attacker rather than a malicious user, e.g. a company that wants to hijack agents into buying their products online.</t>
@@ -58,7 +58,7 @@
 A rather different and serious concern is that long-lived continual learning FMAs may reflect on their goals over time, arrive at a dangerous long-term goal via reflection, and start scheming to pursue that goal.</t>
   </si>
   <si>
-    <t>Pretraining with model architectures that enable recurrent neuralese can lead to neuralese serial reasoning. Outcome-based finetuning, like o1’s, can lead to linguistic drift, jargon, or steganography (especially if there is regularization towards human language). Models could invent jargon or decide to hide their reasoning at runtime, though could likely be detected with monitoring. We may not monitor enough to catch them anyway, because constant monitoring may be very expensive.</t>
+    <t>Pretraining with model architectures that enable recurrent neuralese can lead to neuralese serial reasoning. Outcome-based finetuning, like o1’s, can lead to linguistic drift, jargon, or steganography (steganography being especially plausible if there is regularization towards human language). Models could invent jargon or decide to hide their reasoning at runtime, though could likely be detected with monitoring. We may not monitor enough to catch them anyway, because constant monitoring may be very expensive.</t>
   </si>
   <si>
     <t>In general, development stages that involve training on a numerical feedback signal (such as RL post-training) tend to exacerbate a YGWYM threat model by forcing the training process to distill a complex of relevant goals and values into a single computable metric. 
@@ -101,7 +101,7 @@
     <t>Finetuning</t>
   </si>
   <si>
-    <t>Finetuning can be used for many objectives, including harmlessness and reasoning. Finetuning can lead to undesired outcomes if it offers the system unconstrained exploration (Ross Nordby suggested that RL is concerning when it provides a model with unconstrained exploration opportunities), there are proxies for the specified objective that may be learned instead, or the objective is misspecified (including due to errors in human feedback). This is more likely to lead to large-scale dangerous goals if the intended objective is itself prompt-unconditional. Reasoning finetuning can incentivize hidden serial reasoning.</t>
+    <t>Finetuning can be used for many objectives, including harmlessness and reasoning. Finetuning can lead to undesired outcomes if it offers the system unconstrained exploration, there are proxies for the specified objective that may be learned instead, or the objective is misspecified (including due to errors in human feedback). This is more likely to lead to large-scale dangerous goals if the intended objective is itself prompt-unconditional. Reasoning finetuning can incentivize hidden serial reasoning.</t>
   </si>
   <si>
     <t>Harmlessness finetuning gets models to refuse most (but not all) malicious inputs.
@@ -187,8 +187,7 @@
   </si>
   <si>
     <t>It is unlikely for scaffolding itself to promote hidden serial reasoning, but maybe a user will create a scaffold that encourages a model to do hidden serial reasoning to avoid oversight from elsewhere. For instance, if there are widespread monitoring agents ("police AIs"), and the user doesn't want their agent to get caught doing something, they may include an internal review in their scaffold for whether the police catch the planned behavior.
-Probability: Low?
- Interconnected Components of Scaffolded LLMs/FMAs may develop opaque reasoning patterns.</t>
+Probability: Low?</t>
   </si>
   <si>
     <t>Scaffolding may either increase or reduce the risk of a YGWYM threat model. 
@@ -258,7 +257,7 @@
     <t>Inputs and prompts pick out characters with particular goals.</t>
   </si>
   <si>
-    <t>Learning / reasoning at runtimeRuntime goal-revision / Reflection / Continual Learning</t>
+    <t>Learning / reasoning / goal-revision at runtime</t>
   </si>
   <si>
     <t>Goal-revision could lead to longer-term goals in FMAs. This is something of an X-factor that could break much of the other reasoning in this matrix about where goals come from. Tentatively, and speculatively, it also seems quite plausible that goal-revision is essential for sufficiently powerful (and useful) systems. Scheming, multi-agent threats, and the reduction in probability of pure instruction-following are among the most concerning implications of goal-revision at runtime.</t>

</xml_diff>

<commit_message>
Further content and style improvements, ready to send for feedback
</commit_message>
<xml_diff>
--- a/matrix.xlsx
+++ b/matrix.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Rows: Behavior-shaping mechanisms
 Columns: Qualitative outcomes</t>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>Some properties of agents that may affect multiagent outcomes include their attitudes to risk, negotiation tactics, decision theories, and access to each other’s decision-making processes.</t>
+  </si>
+  <si>
+    <t>Even achieving DWIMAC does not guarantee good outcomes. In particular, DWIMAC is probably compatible with malicious use, multi-agent conflict, international conflict, and value lock-in.</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
         <v>41</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="7"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -999,7 +1002,9 @@
       <c r="H9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="J9" s="7"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>

</xml_diff>